<commit_message>
Fixed progress tracker for 'The Real Numbers and Real Analysis'
</commit_message>
<xml_diff>
--- a/Progress Trackers/Bloch, Ethan - The Real Numbers and Real Analysis.xlsx
+++ b/Progress Trackers/Bloch, Ethan - The Real Numbers and Real Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TeX\Books\Repository\Progress Trackers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA61731-1447-47EE-939B-80ECA6F75C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3879C0BC-6F85-4BC5-A39A-5FFE5C130F14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3A50DCF6-8EC4-4B74-A69E-2F5909F72904}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Status</t>
   </si>
@@ -111,7 +111,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -126,13 +126,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -448,104 +441,104 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A2472A-B02A-47D8-B69B-8CAB460EB257}">
   <dimension ref="A1:CP26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
-      <selection activeCell="CP27" sqref="CP27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:CN26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.7109375" style="1" customWidth="1"/>
     <col min="19" max="19" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.7109375" style="1" customWidth="1"/>
     <col min="21" max="21" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="2.7109375" style="1" customWidth="1"/>
     <col min="23" max="23" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.7109375" style="1" customWidth="1"/>
     <col min="25" max="25" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="2.7109375" style="1" customWidth="1"/>
     <col min="27" max="27" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="2.7109375" style="1" customWidth="1"/>
     <col min="29" max="29" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="2.7109375" style="1" customWidth="1"/>
     <col min="31" max="31" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="2.7109375" style="1" customWidth="1"/>
     <col min="33" max="33" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="2.7109375" style="1" customWidth="1"/>
     <col min="35" max="35" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="2.7109375" style="1" customWidth="1"/>
     <col min="37" max="37" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="2.7109375" style="1" customWidth="1"/>
     <col min="39" max="39" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="2.7109375" style="1" customWidth="1"/>
     <col min="41" max="41" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="2.7109375" style="1" customWidth="1"/>
     <col min="43" max="43" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="2.7109375" style="1" customWidth="1"/>
     <col min="45" max="45" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="2.7109375" style="1" customWidth="1"/>
     <col min="47" max="47" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="2.7109375" style="1" customWidth="1"/>
     <col min="49" max="49" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8" style="1" customWidth="1"/>
+    <col min="50" max="50" width="2.7109375" style="1" customWidth="1"/>
     <col min="51" max="51" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8" style="1" customWidth="1"/>
+    <col min="52" max="52" width="2.7109375" style="1" customWidth="1"/>
     <col min="53" max="53" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8" style="1" customWidth="1"/>
+    <col min="54" max="54" width="2.7109375" style="1" customWidth="1"/>
     <col min="55" max="55" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8" style="1" customWidth="1"/>
+    <col min="56" max="56" width="2.7109375" style="1" customWidth="1"/>
     <col min="57" max="57" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="8" style="1" customWidth="1"/>
+    <col min="58" max="58" width="2.7109375" style="1" customWidth="1"/>
     <col min="59" max="59" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="8" style="1" customWidth="1"/>
+    <col min="60" max="60" width="2.7109375" style="1" customWidth="1"/>
     <col min="61" max="61" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8" style="1" customWidth="1"/>
+    <col min="62" max="62" width="2.7109375" style="1" customWidth="1"/>
     <col min="63" max="63" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8" style="1" customWidth="1"/>
+    <col min="64" max="64" width="2.7109375" style="1" customWidth="1"/>
     <col min="65" max="65" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="8" style="1" customWidth="1"/>
+    <col min="66" max="66" width="2.7109375" style="1" customWidth="1"/>
     <col min="67" max="67" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="8" style="1" customWidth="1"/>
+    <col min="68" max="68" width="2.7109375" style="1" customWidth="1"/>
     <col min="69" max="69" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8" style="1" customWidth="1"/>
+    <col min="70" max="70" width="2.7109375" style="1" customWidth="1"/>
     <col min="71" max="71" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8" style="1" customWidth="1"/>
+    <col min="72" max="72" width="2.7109375" style="1" customWidth="1"/>
     <col min="73" max="73" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="8" style="1" customWidth="1"/>
+    <col min="74" max="74" width="2.7109375" style="1" customWidth="1"/>
     <col min="75" max="75" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="8" style="1" customWidth="1"/>
+    <col min="76" max="76" width="2.7109375" style="1" customWidth="1"/>
     <col min="77" max="77" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="8" style="1" customWidth="1"/>
+    <col min="78" max="78" width="2.7109375" style="1" customWidth="1"/>
     <col min="79" max="79" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="8" style="1" customWidth="1"/>
+    <col min="80" max="80" width="2.7109375" style="1" customWidth="1"/>
     <col min="81" max="81" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="8" style="1" customWidth="1"/>
+    <col min="82" max="82" width="2.7109375" style="1" customWidth="1"/>
     <col min="83" max="83" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="8" style="1" customWidth="1"/>
+    <col min="84" max="84" width="2.7109375" style="1" customWidth="1"/>
     <col min="85" max="85" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="8" style="1" customWidth="1"/>
+    <col min="86" max="86" width="2.7109375" style="1" customWidth="1"/>
     <col min="87" max="87" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="8" style="1" customWidth="1"/>
+    <col min="88" max="88" width="2.7109375" style="1" customWidth="1"/>
     <col min="89" max="89" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="8" style="1" customWidth="1"/>
+    <col min="90" max="90" width="2.7109375" style="1" customWidth="1"/>
     <col min="91" max="91" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="8" style="1" customWidth="1"/>
+    <col min="92" max="92" width="2.7109375" style="1" customWidth="1"/>
     <col min="93" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1214,6 +1207,9 @@
       <c r="BM5" s="1">
         <v>3</v>
       </c>
+      <c r="BN5" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BO5" s="1">
         <v>3</v>
       </c>
@@ -1358,6 +1354,9 @@
       <c r="BM6" s="1">
         <v>4</v>
       </c>
+      <c r="BN6" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BO6" s="1">
         <v>4</v>
       </c>
@@ -2292,7 +2291,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="17:94" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:94" x14ac:dyDescent="0.25">
       <c r="Q17" s="1">
         <v>15</v>
       </c>
@@ -2324,7 +2323,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="17:94" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:94" x14ac:dyDescent="0.25">
       <c r="Q18" s="1">
         <v>16</v>
       </c>
@@ -2353,7 +2352,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="17:94" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:94" x14ac:dyDescent="0.25">
       <c r="Q19" s="1">
         <v>17</v>
       </c>
@@ -2373,7 +2372,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="17:94" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:94" x14ac:dyDescent="0.25">
       <c r="Q20" s="1">
         <v>18</v>
       </c>
@@ -2393,103 +2392,199 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="17:94" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:94" x14ac:dyDescent="0.25">
       <c r="Q21" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="17:94" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:94" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Q22" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="17:94" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:94" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <f t="shared" ref="A23:AW24" si="1">COUNTIF(B$3:B$22,$CO23)</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AH23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AL23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AP23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AR23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AT23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AV23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="AX23" s="3">
         <f>COUNTIF(AX$3:AX$22,$CO23)</f>
         <v>0</v>
       </c>
       <c r="AZ23" s="3">
-        <f t="shared" ref="AY23:CN24" si="1">COUNTIF(AZ$3:AZ$22,$CO23)</f>
+        <f t="shared" ref="AY23:CN24" si="2">COUNTIF(AZ$3:AZ$22,$CO23)</f>
         <v>0</v>
       </c>
       <c r="BB23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BD23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BF23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BH23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BJ23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BL23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BN23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BP23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BR23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BT23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BV23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BX23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BZ23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CB23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CD23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CF23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CH23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CJ23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CL23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CN23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CO23" s="3" t="str">
@@ -2501,93 +2596,189 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="17:94" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:94" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF24" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AH24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AL24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AP24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AR24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AT24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AV24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="AX24" s="3">
         <f>COUNTIF(AX$3:AX$22,$CO24)</f>
         <v>0</v>
       </c>
       <c r="AZ24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BB24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BD24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BF24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BH24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BJ24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BL24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BN24" s="3">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="BP24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BR24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BT24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BV24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BX24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BZ24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CB24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CD24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CF24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CH24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CJ24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CL24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CN24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CO24" s="3" t="str">
@@ -2595,118 +2786,210 @@
         <v>Co</v>
       </c>
       <c r="CP24" s="3">
-        <f t="shared" ref="CP24:CP25" si="2">SUM(AX24:CN24)</f>
-        <v>2</v>
+        <f t="shared" ref="CP24:CP25" si="3">SUM(AX24:CN24)</f>
+        <v>4</v>
       </c>
     </row>
-    <row r="25" spans="17:94" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:94" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
+        <f t="shared" ref="A25:AW25" si="4">B$2</f>
+        <v>8</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="H25" s="3">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="L25" s="3">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="N25" s="3">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="P25" s="3">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="R25" s="3">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="T25" s="3">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="V25" s="3">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="X25" s="3">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="Z25" s="3">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="AB25" s="3">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="AD25" s="3">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="AF25" s="3">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="AH25" s="3">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="AJ25" s="3">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="AL25" s="3">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="AN25" s="3">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="AP25" s="3">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="AR25" s="3">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="AT25" s="3">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="AV25" s="3">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
       <c r="AX25" s="3">
         <f>AX$2</f>
         <v>11</v>
       </c>
       <c r="AZ25" s="3">
-        <f t="shared" ref="AY25:CN25" si="3">AZ$2</f>
+        <f t="shared" ref="AY25:CN25" si="5">AZ$2</f>
         <v>6</v>
       </c>
       <c r="BB25" s="3">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="BD25" s="3">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="BF25" s="3">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="BH25" s="3">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="BJ25" s="3">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="BL25" s="3">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="BN25" s="3">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="BP25" s="3">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="BR25" s="3">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="BT25" s="3">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="BV25" s="3">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="BX25" s="3">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="BZ25" s="3">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="CB25" s="3">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="CD25" s="3">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="CF25" s="3">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="CH25" s="3">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="CJ25" s="3">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="CL25" s="3">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="CN25" s="3">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="CO25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="CP25" s="3">
         <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="BD25" s="3">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="BF25" s="3">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="BH25" s="3">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="BJ25" s="3">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="BL25" s="3">
-        <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
-      <c r="BN25" s="3">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="BP25" s="3">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="BR25" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="BT25" s="3">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="BV25" s="3">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="BX25" s="3">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="BZ25" s="3">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="CB25" s="3">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="CD25" s="3">
-        <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
-      <c r="CF25" s="3">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="CH25" s="3">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="CJ25" s="3">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="CL25" s="3">
-        <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
-      <c r="CN25" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="CO25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="CP25" s="3">
-        <f t="shared" si="2"/>
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="17:94" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="AX26" s="4">
-        <f>AX24/AX25</f>
-        <v>0</v>
-      </c>
+    <row r="26" spans="2:94" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="CO26" s="4" t="s">
         <v>4</v>
       </c>
       <c r="CP26" s="4">
         <f>CP24/CP25</f>
-        <v>8.0321285140562242E-3</v>
+        <v>1.6064257028112448E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2746,7 +3029,7 @@
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4A89454D-85C0-4C01-B01F-BD9CA48FAE01}">
           <x14:formula1>
             <xm:f>Status!$A$2:$A$4</xm:f>

</xml_diff>